<commit_message>
work plan update 06092018
</commit_message>
<xml_diff>
--- a/_Work_Plan & Review Comments.xlsx
+++ b/_Work_Plan & Review Comments.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>Data prep-processing</t>
+  </si>
+  <si>
+    <t>Score Calculation</t>
+  </si>
+  <si>
+    <t>ML model build</t>
+  </si>
+  <si>
+    <t>ML model deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Documentation </t>
+  </si>
+  <si>
+    <t>SparkPython</t>
+  </si>
+  <si>
+    <t>Normal Python</t>
+  </si>
+  <si>
+    <t>Considerations</t>
+  </si>
+  <si>
+    <t>Related code file</t>
+  </si>
+  <si>
+    <t>Deduplication for the bag of words on the payment data level</t>
+  </si>
+  <si>
+    <t>Deduplication for the bag of words on the individual level</t>
+  </si>
+  <si>
+    <t>Deduplication of the failure bag on the payment data level</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,13 +67,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -44,14 +102,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +165,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +200,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +408,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>